<commit_message>
Updated SPI buttons to v1.2
</commit_message>
<xml_diff>
--- a/SPI-Buttons-32/BOM - SPIBUTTONS.xlsx
+++ b/SPI-Buttons-32/BOM - SPIBUTTONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\git\OpenFFBoard-hardware\SPI-Buttons-32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\eagle\projects\shiftregister_buttons\Production\1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C746C2BB-F021-4F79-A00D-B53698BA5132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBA214E-9A7A-49A9-B2BA-2AD3927FB67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="4605" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Comment</t>
   </si>
@@ -51,12 +51,6 @@
     <t>JP3, JP4</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C4</t>
-  </si>
-  <si>
     <t>IC1, IC2, IC3, IC4</t>
   </si>
   <si>
@@ -91,6 +85,45 @@
   </si>
   <si>
     <t>C25804</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4,C8</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R35,R33</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32,R36</t>
+  </si>
+  <si>
+    <t>SN74LVC2G14DBV</t>
+  </si>
+  <si>
+    <t>IC6</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>74LVC1G125DBV</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
+  </si>
+  <si>
+    <t>C12401</t>
+  </si>
+  <si>
+    <t>C23654</t>
+  </si>
+  <si>
+    <t>C21189</t>
   </si>
 </sst>
 </file>
@@ -169,7 +202,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -181,12 +214,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -209,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -355,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -497,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -508,7 +535,7 @@
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -536,80 +563,111 @@
     </row>
     <row r="2" spans="1:4" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>15</v>
+      <c r="A3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
+      <c r="A6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="D9" s="4"/>
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="D10" s="4"/>

</xml_diff>